<commit_message>
added years and added data
</commit_message>
<xml_diff>
--- a/data/sampleData.xlsx
+++ b/data/sampleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="460" windowWidth="10000" windowHeight="14840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2820" yWindow="2600" windowWidth="22120" windowHeight="12680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="105">
   <si>
     <t>date</t>
   </si>
@@ -48,21 +48,12 @@
     <t>EE 468</t>
   </si>
   <si>
-    <t>Operating Systems course</t>
-  </si>
-  <si>
     <t>EE 371</t>
   </si>
   <si>
-    <t>Electromagnetics course</t>
-  </si>
-  <si>
     <t>EE 367</t>
   </si>
   <si>
-    <t>Data Structure and Algorithms course</t>
-  </si>
-  <si>
     <t>Spring 2018</t>
   </si>
   <si>
@@ -90,10 +81,268 @@
     <t>1/8/2018</t>
   </si>
   <si>
-    <t>8/10/2018</t>
-  </si>
-  <si>
-    <t>5/5/2017</t>
+    <t>Fall 2015</t>
+  </si>
+  <si>
+    <t>AMST 150</t>
+  </si>
+  <si>
+    <t>CHEM 171</t>
+  </si>
+  <si>
+    <t>ECON 131</t>
+  </si>
+  <si>
+    <t>MATH 251A</t>
+  </si>
+  <si>
+    <t>America and the World</t>
+  </si>
+  <si>
+    <t>Principles of Chemistry</t>
+  </si>
+  <si>
+    <t>Principles of Macroeconomics</t>
+  </si>
+  <si>
+    <t>Accelerated Calculus I</t>
+  </si>
+  <si>
+    <t>Spring 2016</t>
+  </si>
+  <si>
+    <t>COMG 251</t>
+  </si>
+  <si>
+    <t>EE 160</t>
+  </si>
+  <si>
+    <t>MATH 252A</t>
+  </si>
+  <si>
+    <t>PHYS 170A</t>
+  </si>
+  <si>
+    <t>8/20/2015</t>
+  </si>
+  <si>
+    <t>1/8/2016</t>
+  </si>
+  <si>
+    <t>Principles of Effective Public Speaking</t>
+  </si>
+  <si>
+    <t>Programming for Engineers</t>
+  </si>
+  <si>
+    <t>Accelerated Calculus II</t>
+  </si>
+  <si>
+    <t>General Physics I</t>
+  </si>
+  <si>
+    <t>Fall 2016</t>
+  </si>
+  <si>
+    <t>EE 211</t>
+  </si>
+  <si>
+    <t>EE 260</t>
+  </si>
+  <si>
+    <t>MATH 253A</t>
+  </si>
+  <si>
+    <t>PHYS 272</t>
+  </si>
+  <si>
+    <t>8/20/2016</t>
+  </si>
+  <si>
+    <t>Basic Circuit Analysis I</t>
+  </si>
+  <si>
+    <t>Introduction to Digital Design</t>
+  </si>
+  <si>
+    <t>General Physics II</t>
+  </si>
+  <si>
+    <t>Accelerated Calculus III</t>
+  </si>
+  <si>
+    <t>1/8/2017</t>
+  </si>
+  <si>
+    <t>EE 205</t>
+  </si>
+  <si>
+    <t>EE 213</t>
+  </si>
+  <si>
+    <t>ENGR 296</t>
+  </si>
+  <si>
+    <t>HWST 107</t>
+  </si>
+  <si>
+    <t>MATH 307</t>
+  </si>
+  <si>
+    <t>PHYS 274</t>
+  </si>
+  <si>
+    <t>Object Oriented Programming</t>
+  </si>
+  <si>
+    <t>Basic Circuit Analysis II</t>
+  </si>
+  <si>
+    <t>Sophmore VIP</t>
+  </si>
+  <si>
+    <t>Hawaii: Center of the Pacific</t>
+  </si>
+  <si>
+    <t>Linear Algebra and Differential Equations</t>
+  </si>
+  <si>
+    <t>General Physics III</t>
+  </si>
+  <si>
+    <t>Summer 2017</t>
+  </si>
+  <si>
+    <t>GEOG 151</t>
+  </si>
+  <si>
+    <t>Geography and Contemporary Society</t>
+  </si>
+  <si>
+    <t>Fall 2017</t>
+  </si>
+  <si>
+    <t>8/20/2017</t>
+  </si>
+  <si>
+    <t>EE 315</t>
+  </si>
+  <si>
+    <t>EE 324</t>
+  </si>
+  <si>
+    <t>EE 361</t>
+  </si>
+  <si>
+    <t>EE 362</t>
+  </si>
+  <si>
+    <t>EE 396</t>
+  </si>
+  <si>
+    <t>HON 333</t>
+  </si>
+  <si>
+    <t>Signals and System Analysis</t>
+  </si>
+  <si>
+    <t>Physical Electronics</t>
+  </si>
+  <si>
+    <t>Digital Systems and Computer Design</t>
+  </si>
+  <si>
+    <t>Discrete Math for Engineers</t>
+  </si>
+  <si>
+    <t>Junior Project</t>
+  </si>
+  <si>
+    <t>Junior VIP</t>
+  </si>
+  <si>
+    <t>Experiential Scholoarly Engage</t>
+  </si>
+  <si>
+    <t>EE 323</t>
+  </si>
+  <si>
+    <t>EE 342</t>
+  </si>
+  <si>
+    <t>EE 314</t>
+  </si>
+  <si>
+    <t>MATH 372</t>
+  </si>
+  <si>
+    <t>Microelectronic Circuits I</t>
+  </si>
+  <si>
+    <t>EE Probability and Statistics</t>
+  </si>
+  <si>
+    <t>Computer Data Structure and Algorithms</t>
+  </si>
+  <si>
+    <t>Software Engineering I</t>
+  </si>
+  <si>
+    <t>Elementary Probability and Statistics</t>
+  </si>
+  <si>
+    <t>ICS 414</t>
+  </si>
+  <si>
+    <t>MATH 321</t>
+  </si>
+  <si>
+    <t>Software Engineering II</t>
+  </si>
+  <si>
+    <t>Introduction to Advanced Mathematics</t>
+  </si>
+  <si>
+    <t>Engineering Electromagnetics I</t>
+  </si>
+  <si>
+    <t>Introduction to Operating Systems</t>
+  </si>
+  <si>
+    <t>EE 491D</t>
+  </si>
+  <si>
+    <t>Special Topics in EE: Comm</t>
+  </si>
+  <si>
+    <t>EE 495</t>
+  </si>
+  <si>
+    <t>Ethics in Electrical Engineering</t>
+  </si>
+  <si>
+    <t>EE 496</t>
+  </si>
+  <si>
+    <t>Capstone Design Project</t>
+  </si>
+  <si>
+    <t>ICS 491</t>
+  </si>
+  <si>
+    <t>Special Topics</t>
+  </si>
+  <si>
+    <t>8/1/2018</t>
+  </si>
+  <si>
+    <t>5/1/2017</t>
+  </si>
+  <si>
+    <t>6/1/2017</t>
+  </si>
+  <si>
+    <t>6/1/2018</t>
   </si>
 </sst>
 </file>
@@ -429,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +707,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -467,35 +716,539 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
         <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -507,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,30 +1287,30 @@
     </row>
     <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>